<commit_message>
modify 8888-08-08 to null
</commit_message>
<xml_diff>
--- a/VeloMax/Ressources/Tables/piece.xlsx
+++ b/VeloMax/Ressources/Tables/piece.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quent\Documents\Info\Esilv\S6\BDD\ProjetFinal\VeloMax\Ressources\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCE3A86-267E-46D7-AA67-077AE050A993}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5038AEA-8F2C-4123-A5F4-D9A1D0922F95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>numero_piece_catalogue</t>
   </si>
@@ -148,12 +145,6 @@
   </si>
   <si>
     <t>panier</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>finalQueryGuillemets</t>
   </si>
   <si>
     <t>finalQueryNormal</t>
@@ -227,25 +218,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Feuil1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="J2" t="str">
-            <v>INSERT INTO velo VALUES (1,'Kilimandjaro','Adulte',115,'Classique','2012-01-01','2016-12-01',252);</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -511,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -531,7 +503,7 @@
     <col min="10" max="10" width="23.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -557,16 +529,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="str">
         <f>"RS_"&amp;B2</f>
         <v>RS_P1</v>
@@ -580,9 +546,9 @@
       <c r="D2" s="1">
         <v>40179</v>
       </c>
-      <c r="E2" s="1">
-        <f ca="1">IF(TODAY()-DATE(6,0,0)&gt;=D2,D2+DATE(5,0,0),DATE(8888,8,8))</f>
-        <v>41975</v>
+      <c r="E2" s="1" t="str">
+        <f ca="1">IF(TODAY()-DATE(6,0,0)&gt;=D2,TEXT(D2+DATE(5,0,0),"'aaaa-mm-jj'"),"null")</f>
+        <v>'2014-12-02'</v>
       </c>
       <c r="F2">
         <v>79</v>
@@ -594,18 +560,11 @@
         <v>50</v>
       </c>
       <c r="I2" s="3" t="str">
-        <f t="shared" ref="I2:I21" ca="1" si="0">"INSERT INTO piece VALUES ('"&amp;A2&amp;"','"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;TEXT(D2,"aaaa-mm-jj")&amp;"','"&amp;TEXT(E2,"aaaa-mm-jj")&amp;"',"&amp;F2&amp;","&amp;G2&amp;","&amp;H2&amp;");"</f>
+        <f ca="1">"INSERT INTO piece VALUES ('"&amp;A2&amp;"','"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;TEXT(D2,"aaaa-mm-jj")&amp;"',"&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;","&amp;H2&amp;");"</f>
         <v>INSERT INTO piece VALUES ('RS_P1','P1','cadre','2010-01-01','2014-12-02',79,7,50);</v>
       </c>
-      <c r="J2" t="str">
-        <f ca="1">"INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('"&amp;A2&amp;"','"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;TEXT(D2,"aaaa-mm-jj")&amp;"','"&amp;TEXT(E2,"aaaa-mm-jj")&amp;"',"&amp;F2&amp;","&amp;G2&amp;","&amp;H2&amp;");"</f>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('RS_P1','P1','cadre','2010-01-01','2014-12-02',79,7,50);</v>
-      </c>
-      <c r="K2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="str">
         <f>"Farnell_"&amp;B3</f>
         <v>Farnell_P2</v>
@@ -619,9 +578,9 @@
       <c r="D3" s="1">
         <v>40909</v>
       </c>
-      <c r="E3" s="1">
-        <f t="shared" ref="E3:E21" ca="1" si="1">IF(TODAY()-DATE(6,0,0)&gt;=D3,D3+DATE(5,0,0),DATE(8888,8,8))</f>
-        <v>42705</v>
+      <c r="E3" s="1" t="str">
+        <f t="shared" ref="E3:E21" ca="1" si="0">IF(TODAY()-DATE(6,0,0)&gt;=D3,TEXT(D3+DATE(5,0,0),"'aaaa-mm-jj'"),"null")</f>
+        <v>'2016-12-01'</v>
       </c>
       <c r="F3">
         <v>48</v>
@@ -633,18 +592,11 @@
         <v>120</v>
       </c>
       <c r="I3" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="I3:I21" ca="1" si="1">"INSERT INTO piece VALUES ('"&amp;A3&amp;"','"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;TEXT(D3,"aaaa-mm-jj")&amp;"',"&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;");"</f>
         <v>INSERT INTO piece VALUES ('Farnell_P2','P2','cadre','2012-01-01','2016-12-01',48,25,120);</v>
       </c>
-      <c r="J3" t="str">
-        <f t="shared" ref="J3:J21" ca="1" si="2">"INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('"&amp;A3&amp;"','"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;TEXT(D3,"aaaa-mm-jj")&amp;"','"&amp;TEXT(E3,"aaaa-mm-jj")&amp;"',"&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;");"</f>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('Farnell_P2','P2','cadre','2012-01-01','2016-12-01',48,25,120);</v>
-      </c>
-      <c r="K3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="str">
         <f>"Digikey_"&amp;B4</f>
         <v>Digikey_P3</v>
@@ -658,9 +610,9 @@
       <c r="D4" s="1">
         <v>42736</v>
       </c>
-      <c r="E4" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>2552537</v>
+      <c r="E4" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>null</v>
       </c>
       <c r="F4">
         <v>126</v>
@@ -672,18 +624,11 @@
         <v>30</v>
       </c>
       <c r="I4" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO piece VALUES ('Digikey_P3','P3','cadre','2017-01-01','8888-08-08',126,25,30);</v>
-      </c>
-      <c r="J4" t="str">
-        <f ca="1">"INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('"&amp;A4&amp;"','"&amp;B4&amp;"','"&amp;C4&amp;"','"&amp;TEXT(D4,"aaaa-mm-jj")&amp;"','"&amp;[1]Feuil1!$J$2&amp;"',"&amp;F4&amp;","&amp;G4&amp;","&amp;H4&amp;");"</f>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('Digikey_P3','P3','cadre','2017-01-01','INSERT INTO velo VALUES (1,'Kilimandjaro','Adulte',115,'Classique','2012-01-01','2016-12-01',252);',126,25,30);</v>
-      </c>
-      <c r="K4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO piece VALUES ('Digikey_P3','P3','cadre','2017-01-01',null,126,25,30);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="str">
         <f>"Mouser_"&amp;B5</f>
         <v>Mouser_P4</v>
@@ -697,9 +642,9 @@
       <c r="D5" s="1">
         <v>43831</v>
       </c>
-      <c r="E5" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>2552537</v>
+      <c r="E5" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>null</v>
       </c>
       <c r="F5">
         <v>29</v>
@@ -711,20 +656,13 @@
         <v>20</v>
       </c>
       <c r="I5" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO piece VALUES ('Mouser_P4','P4','cadre','2020-01-01','8888-08-08',29,25,20);</v>
-      </c>
-      <c r="J5" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('Mouser_P4','P4','cadre','2020-01-01','8888-08-08',29,25,20);</v>
-      </c>
-      <c r="K5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO piece VALUES ('Mouser_P4','P4','cadre','2020-01-01',null,29,25,20);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="str">
-        <f t="shared" ref="A6" si="3">"RS_"&amp;B6</f>
+        <f t="shared" ref="A6" si="2">"RS_"&amp;B6</f>
         <v>RS_P5</v>
       </c>
       <c r="B6" t="s">
@@ -736,9 +674,9 @@
       <c r="D6" s="1">
         <v>40179</v>
       </c>
-      <c r="E6" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>41975</v>
+      <c r="E6" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>'2014-12-02'</v>
       </c>
       <c r="F6">
         <v>30</v>
@@ -750,20 +688,13 @@
         <v>40</v>
       </c>
       <c r="I6" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>INSERT INTO piece VALUES ('RS_P5','P5','guidon','2010-01-01','2014-12-02',30,90,40);</v>
       </c>
-      <c r="J6" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('RS_P5','P5','guidon','2010-01-01','2014-12-02',30,90,40);</v>
-      </c>
-      <c r="K6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="str">
-        <f t="shared" ref="A7" si="4">"Farnell_"&amp;B7</f>
+        <f t="shared" ref="A7" si="3">"Farnell_"&amp;B7</f>
         <v>Farnell_P6</v>
       </c>
       <c r="B7" t="s">
@@ -775,9 +706,9 @@
       <c r="D7" s="1">
         <v>40909</v>
       </c>
-      <c r="E7" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>42705</v>
+      <c r="E7" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>'2016-12-01'</v>
       </c>
       <c r="F7">
         <v>56</v>
@@ -789,20 +720,13 @@
         <v>40</v>
       </c>
       <c r="I7" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>INSERT INTO piece VALUES ('Farnell_P6','P6','guidon','2012-01-01','2016-12-01',56,1,40);</v>
       </c>
-      <c r="J7" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('Farnell_P6','P6','guidon','2012-01-01','2016-12-01',56,1,40);</v>
-      </c>
-      <c r="K7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="str">
-        <f t="shared" ref="A8" si="5">"Digikey_"&amp;B8</f>
+        <f t="shared" ref="A8" si="4">"Digikey_"&amp;B8</f>
         <v>Digikey_P7</v>
       </c>
       <c r="B8" t="s">
@@ -814,9 +738,9 @@
       <c r="D8" s="1">
         <v>42736</v>
       </c>
-      <c r="E8" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>2552537</v>
+      <c r="E8" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>null</v>
       </c>
       <c r="F8">
         <v>40</v>
@@ -828,20 +752,13 @@
         <v>40</v>
       </c>
       <c r="I8" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO piece VALUES ('Digikey_P7','P7','guidon','2017-01-01','8888-08-08',40,3,40);</v>
-      </c>
-      <c r="J8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('Digikey_P7','P7','guidon','2017-01-01','8888-08-08',40,3,40);</v>
-      </c>
-      <c r="K8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO piece VALUES ('Digikey_P7','P7','guidon','2017-01-01',null,40,3,40);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="str">
-        <f t="shared" ref="A9" si="6">"Mouser_"&amp;B9</f>
+        <f t="shared" ref="A9" si="5">"Mouser_"&amp;B9</f>
         <v>Mouser_P8</v>
       </c>
       <c r="B9" t="s">
@@ -853,9 +770,9 @@
       <c r="D9" s="1">
         <v>40179</v>
       </c>
-      <c r="E9" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>41975</v>
+      <c r="E9" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>'2014-12-02'</v>
       </c>
       <c r="F9">
         <v>119</v>
@@ -867,20 +784,13 @@
         <v>20</v>
       </c>
       <c r="I9" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>INSERT INTO piece VALUES ('Mouser_P8','P8','freins','2010-01-01','2014-12-02',119,5,20);</v>
       </c>
-      <c r="J9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('Mouser_P8','P8','freins','2010-01-01','2014-12-02',119,5,20);</v>
-      </c>
-      <c r="K9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="str">
-        <f t="shared" ref="A10" si="7">"RS_"&amp;B10</f>
+        <f t="shared" ref="A10" si="6">"RS_"&amp;B10</f>
         <v>RS_P9</v>
       </c>
       <c r="B10" t="s">
@@ -892,9 +802,9 @@
       <c r="D10" s="1">
         <v>40909</v>
       </c>
-      <c r="E10" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>42705</v>
+      <c r="E10" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>'2016-12-01'</v>
       </c>
       <c r="F10">
         <v>48</v>
@@ -906,20 +816,13 @@
         <v>35</v>
       </c>
       <c r="I10" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>INSERT INTO piece VALUES ('RS_P9','P9','freins','2012-01-01','2016-12-01',48,1,35);</v>
       </c>
-      <c r="J10" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('RS_P9','P9','freins','2012-01-01','2016-12-01',48,1,35);</v>
-      </c>
-      <c r="K10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="str">
-        <f t="shared" ref="A11" si="8">"Farnell_"&amp;B11</f>
+        <f t="shared" ref="A11" si="7">"Farnell_"&amp;B11</f>
         <v>Farnell_P10</v>
       </c>
       <c r="B11" t="s">
@@ -931,9 +834,9 @@
       <c r="D11" s="1">
         <v>42736</v>
       </c>
-      <c r="E11" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>2552537</v>
+      <c r="E11" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>null</v>
       </c>
       <c r="F11">
         <v>18</v>
@@ -945,20 +848,13 @@
         <v>50</v>
       </c>
       <c r="I11" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO piece VALUES ('Farnell_P10','P10','freins','2017-01-01','8888-08-08',18,3,50);</v>
-      </c>
-      <c r="J11" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('Farnell_P10','P10','freins','2017-01-01','8888-08-08',18,3,50);</v>
-      </c>
-      <c r="K11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO piece VALUES ('Farnell_P10','P10','freins','2017-01-01',null,18,3,50);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="str">
-        <f t="shared" ref="A12" si="9">"Digikey_"&amp;B12</f>
+        <f t="shared" ref="A12" si="8">"Digikey_"&amp;B12</f>
         <v>Digikey_P11</v>
       </c>
       <c r="B12" t="s">
@@ -970,9 +866,9 @@
       <c r="D12" s="1">
         <v>40179</v>
       </c>
-      <c r="E12" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>41975</v>
+      <c r="E12" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>'2014-12-02'</v>
       </c>
       <c r="F12">
         <v>32</v>
@@ -984,20 +880,13 @@
         <v>200</v>
       </c>
       <c r="I12" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>INSERT INTO piece VALUES ('Digikey_P11','P11','selle','2010-01-01','2014-12-02',32,7,200);</v>
       </c>
-      <c r="J12" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('Digikey_P11','P11','selle','2010-01-01','2014-12-02',32,7,200);</v>
-      </c>
-      <c r="K12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="str">
-        <f t="shared" ref="A13" si="10">"Mouser_"&amp;B13</f>
+        <f t="shared" ref="A13" si="9">"Mouser_"&amp;B13</f>
         <v>Mouser_P12</v>
       </c>
       <c r="B13" t="s">
@@ -1009,9 +898,9 @@
       <c r="D13" s="1">
         <v>40179</v>
       </c>
-      <c r="E13" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>41975</v>
+      <c r="E13" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>'2014-12-02'</v>
       </c>
       <c r="F13">
         <v>25</v>
@@ -1023,20 +912,13 @@
         <v>180</v>
       </c>
       <c r="I13" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>INSERT INTO piece VALUES ('Mouser_P12','P12','derailleur avant','2010-01-01','2014-12-02',25,15,180);</v>
       </c>
-      <c r="J13" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('Mouser_P12','P12','derailleur avant','2010-01-01','2014-12-02',25,15,180);</v>
-      </c>
-      <c r="K13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="str">
-        <f t="shared" ref="A14" si="11">"RS_"&amp;B14</f>
+        <f t="shared" ref="A14" si="10">"RS_"&amp;B14</f>
         <v>RS_P13</v>
       </c>
       <c r="B14" t="s">
@@ -1048,9 +930,9 @@
       <c r="D14" s="1">
         <v>40179</v>
       </c>
-      <c r="E14" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>41975</v>
+      <c r="E14" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>'2014-12-02'</v>
       </c>
       <c r="F14">
         <v>20</v>
@@ -1062,20 +944,13 @@
         <v>180</v>
       </c>
       <c r="I14" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>INSERT INTO piece VALUES ('RS_P13','P13','derailleur arriere','2010-01-01','2014-12-02',20,90,180);</v>
       </c>
-      <c r="J14" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('RS_P13','P13','derailleur arriere','2010-01-01','2014-12-02',20,90,180);</v>
-      </c>
-      <c r="K14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="str">
-        <f t="shared" ref="A15" si="12">"Farnell_"&amp;B15</f>
+        <f t="shared" ref="A15" si="11">"Farnell_"&amp;B15</f>
         <v>Farnell_P14</v>
       </c>
       <c r="B15" t="s">
@@ -1087,9 +962,9 @@
       <c r="D15" s="1">
         <v>40179</v>
       </c>
-      <c r="E15" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>41975</v>
+      <c r="E15" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>'2014-12-02'</v>
       </c>
       <c r="F15">
         <v>55</v>
@@ -1101,20 +976,13 @@
         <v>220</v>
       </c>
       <c r="I15" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>INSERT INTO piece VALUES ('Farnell_P14','P14','roue avant','2010-01-01','2014-12-02',55,5,220);</v>
       </c>
-      <c r="J15" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('Farnell_P14','P14','roue avant','2010-01-01','2014-12-02',55,5,220);</v>
-      </c>
-      <c r="K15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="str">
-        <f t="shared" ref="A16" si="13">"Digikey_"&amp;B16</f>
+        <f t="shared" ref="A16" si="12">"Digikey_"&amp;B16</f>
         <v>Digikey_P15</v>
       </c>
       <c r="B16" t="s">
@@ -1126,9 +994,9 @@
       <c r="D16" s="1">
         <v>40909</v>
       </c>
-      <c r="E16" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>42705</v>
+      <c r="E16" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>'2016-12-01'</v>
       </c>
       <c r="F16">
         <v>32</v>
@@ -1140,20 +1008,13 @@
         <v>200</v>
       </c>
       <c r="I16" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>INSERT INTO piece VALUES ('Digikey_P15','P15','roue avant','2012-01-01','2016-12-01',32,1,200);</v>
       </c>
-      <c r="J16" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('Digikey_P15','P15','roue avant','2012-01-01','2016-12-01',32,1,200);</v>
-      </c>
-      <c r="K16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="str">
-        <f t="shared" ref="A17" si="14">"Mouser_"&amp;B17</f>
+        <f t="shared" ref="A17" si="13">"Mouser_"&amp;B17</f>
         <v>Mouser_P16</v>
       </c>
       <c r="B17" t="s">
@@ -1165,9 +1026,9 @@
       <c r="D17" s="1">
         <v>40179</v>
       </c>
-      <c r="E17" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>41975</v>
+      <c r="E17" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>'2014-12-02'</v>
       </c>
       <c r="F17">
         <v>63</v>
@@ -1179,20 +1040,13 @@
         <v>400</v>
       </c>
       <c r="I17" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>INSERT INTO piece VALUES ('Mouser_P16','P16','roue arriere','2010-01-01','2014-12-02',63,15,400);</v>
       </c>
-      <c r="J17" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('Mouser_P16','P16','roue arriere','2010-01-01','2014-12-02',63,15,400);</v>
-      </c>
-      <c r="K17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="str">
-        <f t="shared" ref="A18" si="15">"RS_"&amp;B18</f>
+        <f t="shared" ref="A18" si="14">"RS_"&amp;B18</f>
         <v>RS_P17</v>
       </c>
       <c r="B18" t="s">
@@ -1204,9 +1058,9 @@
       <c r="D18" s="1">
         <v>40179</v>
       </c>
-      <c r="E18" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>41975</v>
+      <c r="E18" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>'2014-12-02'</v>
       </c>
       <c r="F18">
         <v>9</v>
@@ -1218,20 +1072,13 @@
         <v>1000</v>
       </c>
       <c r="I18" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>INSERT INTO piece VALUES ('RS_P17','P17','reflecteurs','2010-01-01','2014-12-02',9,3,1000);</v>
       </c>
-      <c r="J18" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('RS_P17','P17','reflecteurs','2010-01-01','2014-12-02',9,3,1000);</v>
-      </c>
-      <c r="K18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="str">
-        <f t="shared" ref="A19" si="16">"Farnell_"&amp;B19</f>
+        <f t="shared" ref="A19" si="15">"Farnell_"&amp;B19</f>
         <v>Farnell_P18</v>
       </c>
       <c r="B19" t="s">
@@ -1243,9 +1090,9 @@
       <c r="D19" s="1">
         <v>40179</v>
       </c>
-      <c r="E19" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>41975</v>
+      <c r="E19" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>'2014-12-02'</v>
       </c>
       <c r="F19">
         <v>38</v>
@@ -1257,20 +1104,13 @@
         <v>120</v>
       </c>
       <c r="I19" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>INSERT INTO piece VALUES ('Farnell_P18','P18','pedalier','2010-01-01','2014-12-02',38,2,120);</v>
       </c>
-      <c r="J19" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('Farnell_P18','P18','pedalier','2010-01-01','2014-12-02',38,2,120);</v>
-      </c>
-      <c r="K19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="str">
-        <f t="shared" ref="A20" si="17">"Digikey_"&amp;B20</f>
+        <f t="shared" ref="A20" si="16">"Digikey_"&amp;B20</f>
         <v>Digikey_P19</v>
       </c>
       <c r="B20" t="s">
@@ -1282,9 +1122,9 @@
       <c r="D20" s="1">
         <v>40179</v>
       </c>
-      <c r="E20" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>41975</v>
+      <c r="E20" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>'2014-12-02'</v>
       </c>
       <c r="F20">
         <v>179</v>
@@ -1296,20 +1136,13 @@
         <v>50</v>
       </c>
       <c r="I20" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>INSERT INTO piece VALUES ('Digikey_P19','P19','ordinateur','2010-01-01','2014-12-02',179,90,50);</v>
       </c>
-      <c r="J20" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('Digikey_P19','P19','ordinateur','2010-01-01','2014-12-02',179,90,50);</v>
-      </c>
-      <c r="K20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="str">
-        <f t="shared" ref="A21" si="18">"Mouser_"&amp;B21</f>
+        <f t="shared" ref="A21" si="17">"Mouser_"&amp;B21</f>
         <v>Mouser_P20</v>
       </c>
       <c r="B21" t="s">
@@ -1321,9 +1154,9 @@
       <c r="D21" s="1">
         <v>40179</v>
       </c>
-      <c r="E21" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>41975</v>
+      <c r="E21" s="1" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>'2014-12-02'</v>
       </c>
       <c r="F21">
         <v>14</v>
@@ -1335,45 +1168,44 @@
         <v>70</v>
       </c>
       <c r="I21" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>INSERT INTO piece VALUES ('Mouser_P20','P20','panier','2010-01-01','2014-12-02',14,2,70);</v>
       </c>
-      <c r="J21" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>INSERT INTO VeloMax.piece (`numero_piece_catalogue`,`numero_piece`,`description_piece`,`date_introduction_piece`,`date_discontinuation_piece`,`prix_piece`,`delai_approvisionnement_piece`,`stock_piece`) VALUES ('Mouser_P20','P20','panier','2010-01-01','2014-12-02',14,2,70);</v>
-      </c>
-      <c r="K21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="E23" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <f ca="1">IF(TODAY()-DATE(6,0,0)&gt;=D2,D2+DATE(5,0,0),DATE(8888,8,8))</f>
+        <v>41975</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>

</xml_diff>